<commit_message>
improvement to nutrient loss modelling:
</commit_message>
<xml_diff>
--- a/data/Model inputs.xlsx
+++ b/data/Model inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexSharples\Projects\meihawai\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0B9167-CC8B-4D00-BCDB-0E73A128258A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DB51A5-E3FD-4ED3-B7D2-6B0274F530FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{D6F8230E-8423-4B85-B552-FD231E74B92D}"/>
+    <workbookView xWindow="57490" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{D6F8230E-8423-4B85-B552-FD231E74B92D}"/>
   </bookViews>
   <sheets>
     <sheet name="land_use_parameters" sheetId="2" r:id="rId1"/>
@@ -29,6 +29,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">dairy_typology!$A$1:$Q$461</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">land_use_parameters!$A$1:$AL$23</definedName>
     <definedName name="prod_cap_scalar">5</definedName>
     <definedName name="solver_adj" localSheetId="7" hidden="1">extension!$C$2:$C$5</definedName>
     <definedName name="solver_cvg" localSheetId="7" hidden="1">0.0001</definedName>
@@ -84,6 +85,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={C60B21D3-0B2D-434C-8550-F53AFEF921F1}</author>
     <author>tc={3B879465-BEBA-4E09-A81F-6CC9C252E0FA}</author>
     <author>tc={B4A8D8AC-5345-4E28-A8CE-72319599675F}</author>
     <author>tc={0245FD7B-BEB9-42BE-8995-AFA36FE384F2}</author>
@@ -93,7 +95,15 @@
     <author>tc={1E64728B-797C-429B-B148-9BD4DACDECC1}</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{3B879465-BEBA-4E09-A81F-6CC9C252E0FA}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{C60B21D3-0B2D-434C-8550-F53AFEF921F1}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Max mitigation cost scaled for each land use to have similar marginal costs for first kg mitigated, with dairy=1000 as reference point.</t>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="1" shapeId="0" xr:uid="{3B879465-BEBA-4E09-A81F-6CC9C252E0FA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -103,7 +113,7 @@
 Sheep/Beef: 12.84 tCO2e per ton meat processed, $5.2/kg meat (benchmark data revenue over 125kg/ha production from annual report) gives ~ 2.14 kg CO2e methane per dollar revenue</t>
       </text>
     </comment>
-    <comment ref="I1" authorId="1" shapeId="0" xr:uid="{B4A8D8AC-5345-4E28-A8CE-72319599675F}">
+    <comment ref="I1" authorId="2" shapeId="0" xr:uid="{B4A8D8AC-5345-4E28-A8CE-72319599675F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -111,7 +121,7 @@
     Makes the horticulture profit curves work properly, agents behave as if they have 0.5 lower capability, preserves the correct relationship between absolute capability and horticulture returns</t>
       </text>
     </comment>
-    <comment ref="Y5" authorId="2" shapeId="0" xr:uid="{0245FD7B-BEB9-42BE-8995-AFA36FE384F2}">
+    <comment ref="Y5" authorId="3" shapeId="0" xr:uid="{0245FD7B-BEB9-42BE-8995-AFA36FE384F2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -119,7 +129,7 @@
     Range is $200,000 to $500,000 with the latter being a 'covered' farm</t>
       </text>
     </comment>
-    <comment ref="M16" authorId="3" shapeId="0" xr:uid="{A07C0877-1E80-4B89-8EC3-5AEF15E1032E}">
+    <comment ref="M16" authorId="4" shapeId="0" xr:uid="{A07C0877-1E80-4B89-8EC3-5AEF15E1032E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -128,7 +138,7 @@
 assumes 1180/ha/year additional fixed cost per 2022 numbers quoted in above</t>
       </text>
     </comment>
-    <comment ref="Y16" authorId="4" shapeId="0" xr:uid="{26DCDBBD-3E74-46AB-84F1-C3A49D53DFB6}">
+    <comment ref="Y16" authorId="5" shapeId="0" xr:uid="{26DCDBBD-3E74-46AB-84F1-C3A49D53DFB6}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -137,7 +147,7 @@
 Also agrees with https://www.nzherald.co.nz/nz/the-price-of-water/MO6MEKBUEKSPTUJH22XAVNNFTU/</t>
       </text>
     </comment>
-    <comment ref="J20" authorId="5" shapeId="0" xr:uid="{D1CAC720-C273-4AEE-843F-C09E692D4AC1}">
+    <comment ref="J20" authorId="6" shapeId="0" xr:uid="{D1CAC720-C273-4AEE-843F-C09E692D4AC1}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -146,7 +156,7 @@
 source on 45k number: </t>
       </text>
     </comment>
-    <comment ref="A23" authorId="6" shapeId="0" xr:uid="{1E64728B-797C-429B-B148-9BD4DACDECC1}">
+    <comment ref="A23" authorId="7" shapeId="0" xr:uid="{1E64728B-797C-429B-B148-9BD4DACDECC1}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1021,7 +1031,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1224,6 +1234,12 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="35">
@@ -1581,7 +1597,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1617,7 +1633,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="42" applyFill="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1982,6 +1997,9 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="G1" dT="2024-05-09T04:07:38.85" personId="{118CCBAE-EC1D-4113-9E61-BFB81BE11111}" id="{C60B21D3-0B2D-434C-8550-F53AFEF921F1}">
+    <text>Max mitigation cost scaled for each land use to have similar marginal costs for first kg mitigated, with dairy=1000 as reference point.</text>
+  </threadedComment>
   <threadedComment ref="H1" dT="2024-03-21T22:43:40.34" personId="{118CCBAE-EC1D-4113-9E61-BFB81BE11111}" id="{3B879465-BEBA-4E09-A81F-6CC9C252E0FA}">
     <text>Calculated as a methane emissions factor per dollar revenue, based on MPI emissions factors cited in Greenhalgh impacts of CC mitigation policies. 
 Dairy: 8.18 tCO2e per t milk solids, $7.79/kgMS gives ~1.1 kg co2e from methane per dollar revenue
@@ -2154,8 +2172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58C23377-C778-4880-BC2A-D4FFA818EEF4}">
   <dimension ref="A1:AL23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U30" sqref="U30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2310,7 +2328,7 @@
         <v>154</v>
       </c>
       <c r="G2">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -2399,7 +2417,7 @@
         <v>154</v>
       </c>
       <c r="G3">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -2520,7 +2538,7 @@
         <v>154</v>
       </c>
       <c r="G4">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -2641,7 +2659,7 @@
         <v>154</v>
       </c>
       <c r="G5">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -2762,7 +2780,7 @@
         <v>154</v>
       </c>
       <c r="G6">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -2883,7 +2901,7 @@
         <v>154</v>
       </c>
       <c r="G7">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -3604,7 +3622,7 @@
         <v>154</v>
       </c>
       <c r="G13">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -3725,7 +3743,7 @@
         <v>154</v>
       </c>
       <c r="G14">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -4012,7 +4030,7 @@
         <v>155</v>
       </c>
       <c r="G17">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="H17">
         <v>2.4700000000000002</v>
@@ -4213,7 +4231,7 @@
         <v>155</v>
       </c>
       <c r="G19">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="H19">
         <f>H17*0.3</f>
@@ -12466,8 +12484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AAA01F1-3803-442D-95FE-AA30B98BA3F6}">
   <dimension ref="A1:Q461"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A427" workbookViewId="0">
-      <selection activeCell="S446" sqref="S446"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="S78" sqref="S78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -12523,10 +12541,10 @@
       <c r="O1" t="s">
         <v>132</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="P1" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="Q1" s="27" t="s">
+      <c r="Q1" s="19" t="s">
         <v>182</v>
       </c>
     </row>
@@ -12571,10 +12589,10 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0.73426684741976689</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O2">
-        <v>0.36086076464668171</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P2">
         <v>1</v>
@@ -12624,10 +12642,10 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.65139438398943228</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O3">
-        <v>0.38303397533001515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P3">
         <v>1</v>
@@ -12677,10 +12695,10 @@
         <v>0</v>
       </c>
       <c r="N4">
-        <v>0.58177137676443924</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O4">
-        <v>0.38945139302494869</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P4">
         <v>1</v>
@@ -12730,10 +12748,10 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O5">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P5">
         <v>1</v>
@@ -12783,10 +12801,10 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.35930258940223547</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O6">
-        <v>0.41103799617915515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P6">
         <v>1</v>
@@ -12836,10 +12854,10 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O7">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P7">
         <v>1</v>
@@ -12889,10 +12907,10 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>0.64831027719689605</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O8">
-        <v>0.62341807401314386</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P8">
         <v>1</v>
@@ -12942,10 +12960,10 @@
         <v>0</v>
       </c>
       <c r="N9">
-        <v>0.4448676725204056</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O9">
-        <v>0.41531041305960925</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P9">
         <v>1</v>
@@ -12995,10 +13013,10 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0.52352941176470591</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O10">
-        <v>0.50251470435144707</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P10">
         <v>1</v>
@@ -13048,10 +13066,10 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0.51018761824679415</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O11">
-        <v>0.57588816480975402</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P11">
         <v>1</v>
@@ -13101,10 +13119,10 @@
         <v>0</v>
       </c>
       <c r="N12">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O12">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P12">
         <v>1</v>
@@ -13154,10 +13172,10 @@
         <v>0</v>
       </c>
       <c r="N13">
-        <v>0.45824967357295954</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O13">
-        <v>0.51320335146725959</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P13">
         <v>1</v>
@@ -13207,10 +13225,10 @@
         <v>0</v>
       </c>
       <c r="N14">
-        <v>0.76547381653636815</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O14">
-        <v>0.62342333215136003</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P14">
         <v>1</v>
@@ -13260,10 +13278,10 @@
         <v>0</v>
       </c>
       <c r="N15">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O15">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P15">
         <v>1</v>
@@ -13313,10 +13331,10 @@
         <v>0</v>
       </c>
       <c r="N16">
-        <v>0.5183350138918108</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O16">
-        <v>0.40189685832839361</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P16">
         <v>1</v>
@@ -13366,10 +13384,10 @@
         <v>0</v>
       </c>
       <c r="N17">
-        <v>0.49311216913983535</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O17">
-        <v>0.45596609720566816</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P17">
         <v>1</v>
@@ -13419,10 +13437,10 @@
         <v>0</v>
       </c>
       <c r="N18">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O18">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P18">
         <v>1</v>
@@ -13472,10 +13490,10 @@
         <v>0</v>
       </c>
       <c r="N19">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O19">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P19">
         <v>1</v>
@@ -13525,10 +13543,10 @@
         <v>0</v>
       </c>
       <c r="N20">
-        <v>0.74238993663655861</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O20">
-        <v>0.53287461773700306</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P20">
         <v>1</v>
@@ -13578,10 +13596,10 @@
         <v>0</v>
       </c>
       <c r="N21">
-        <v>0.84562439327596528</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O21">
-        <v>0.69700323243260454</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P21">
         <v>1</v>
@@ -13631,10 +13649,10 @@
         <v>0</v>
       </c>
       <c r="N22">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O22">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P22">
         <v>1</v>
@@ -13684,10 +13702,10 @@
         <v>0</v>
       </c>
       <c r="N23">
-        <v>0.54974923912371776</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O23">
-        <v>0.39400774523132698</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P23">
         <v>1</v>
@@ -13737,10 +13755,10 @@
         <v>0</v>
       </c>
       <c r="N24">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O24">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P24">
         <v>1</v>
@@ -13790,10 +13808,10 @@
         <v>0</v>
       </c>
       <c r="N25">
-        <v>0.73426684741976689</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O25">
-        <v>0.36086076464668171</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P25">
         <v>1</v>
@@ -13843,10 +13861,10 @@
         <v>0</v>
       </c>
       <c r="N26">
-        <v>0.65139438398943228</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O26">
-        <v>0.38303397533001515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P26">
         <v>1</v>
@@ -13896,10 +13914,10 @@
         <v>0</v>
       </c>
       <c r="N27">
-        <v>0.58177137676443924</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O27">
-        <v>0.38945139302494869</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P27">
         <v>1</v>
@@ -13949,10 +13967,10 @@
         <v>0</v>
       </c>
       <c r="N28">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O28">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P28">
         <v>1</v>
@@ -14002,10 +14020,10 @@
         <v>0</v>
       </c>
       <c r="N29">
-        <v>0.35930258940223547</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O29">
-        <v>0.41103799617915515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P29">
         <v>1</v>
@@ -14055,10 +14073,10 @@
         <v>0</v>
       </c>
       <c r="N30">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O30">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P30">
         <v>1</v>
@@ -14108,10 +14126,10 @@
         <v>0</v>
       </c>
       <c r="N31">
-        <v>0.64831027719689605</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O31">
-        <v>0.62341807401314386</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P31">
         <v>1</v>
@@ -14161,10 +14179,10 @@
         <v>0</v>
       </c>
       <c r="N32">
-        <v>0.4448676725204056</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O32">
-        <v>0.41531041305960925</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P32">
         <v>1</v>
@@ -14214,10 +14232,10 @@
         <v>0</v>
       </c>
       <c r="N33">
-        <v>0.52352941176470591</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O33">
-        <v>0.50251470435144707</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P33">
         <v>1</v>
@@ -14267,10 +14285,10 @@
         <v>0</v>
       </c>
       <c r="N34">
-        <v>0.51018761824679415</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O34">
-        <v>0.57588816480975402</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P34">
         <v>1</v>
@@ -14320,10 +14338,10 @@
         <v>0</v>
       </c>
       <c r="N35">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O35">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P35">
         <v>1</v>
@@ -14373,10 +14391,10 @@
         <v>0</v>
       </c>
       <c r="N36">
-        <v>0.45824967357295954</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O36">
-        <v>0.51320335146725959</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P36">
         <v>1</v>
@@ -14426,10 +14444,10 @@
         <v>0</v>
       </c>
       <c r="N37">
-        <v>0.76547381653636815</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O37">
-        <v>0.62342333215136003</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P37">
         <v>1</v>
@@ -14479,10 +14497,10 @@
         <v>0</v>
       </c>
       <c r="N38">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O38">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P38">
         <v>1</v>
@@ -14532,10 +14550,10 @@
         <v>0</v>
       </c>
       <c r="N39">
-        <v>0.5183350138918108</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O39">
-        <v>0.40189685832839361</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P39">
         <v>1</v>
@@ -14585,10 +14603,10 @@
         <v>0</v>
       </c>
       <c r="N40">
-        <v>0.49311216913983535</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O40">
-        <v>0.45596609720566816</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P40">
         <v>1</v>
@@ -14638,10 +14656,10 @@
         <v>0</v>
       </c>
       <c r="N41">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O41">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P41">
         <v>1</v>
@@ -14691,10 +14709,10 @@
         <v>0</v>
       </c>
       <c r="N42">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O42">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P42">
         <v>1</v>
@@ -14744,10 +14762,10 @@
         <v>0</v>
       </c>
       <c r="N43">
-        <v>0.74238993663655861</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O43">
-        <v>0.53287461773700306</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P43">
         <v>1</v>
@@ -14797,10 +14815,10 @@
         <v>0</v>
       </c>
       <c r="N44">
-        <v>0.84562439327596528</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O44">
-        <v>0.69700323243260454</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P44">
         <v>1</v>
@@ -14850,10 +14868,10 @@
         <v>0</v>
       </c>
       <c r="N45">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O45">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P45">
         <v>1</v>
@@ -14903,10 +14921,10 @@
         <v>0</v>
       </c>
       <c r="N46">
-        <v>0.54974923912371776</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O46">
-        <v>0.39400774523132698</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P46">
         <v>1</v>
@@ -14956,10 +14974,10 @@
         <v>0</v>
       </c>
       <c r="N47">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O47">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P47">
         <v>1</v>
@@ -15009,10 +15027,10 @@
         <v>0</v>
       </c>
       <c r="N48">
-        <v>0.73426684741976689</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O48">
-        <v>0.36086076464668171</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P48">
         <v>1</v>
@@ -15062,10 +15080,10 @@
         <v>0</v>
       </c>
       <c r="N49">
-        <v>0.65139438398943228</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O49">
-        <v>0.38303397533001515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P49">
         <v>1</v>
@@ -15115,10 +15133,10 @@
         <v>0</v>
       </c>
       <c r="N50">
-        <v>0.58177137676443924</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O50">
-        <v>0.38945139302494869</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P50">
         <v>1</v>
@@ -15168,10 +15186,10 @@
         <v>0</v>
       </c>
       <c r="N51">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O51">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P51">
         <v>1</v>
@@ -15221,10 +15239,10 @@
         <v>0</v>
       </c>
       <c r="N52">
-        <v>0.35930258940223547</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O52">
-        <v>0.41103799617915515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P52">
         <v>1</v>
@@ -15274,10 +15292,10 @@
         <v>0</v>
       </c>
       <c r="N53">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O53">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P53">
         <v>1</v>
@@ -15327,10 +15345,10 @@
         <v>0</v>
       </c>
       <c r="N54">
-        <v>0.64831027719689605</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O54">
-        <v>0.62341807401314386</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P54">
         <v>1</v>
@@ -15380,10 +15398,10 @@
         <v>0</v>
       </c>
       <c r="N55">
-        <v>0.4448676725204056</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O55">
-        <v>0.41531041305960925</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P55">
         <v>1</v>
@@ -15433,10 +15451,10 @@
         <v>0</v>
       </c>
       <c r="N56">
-        <v>0.52352941176470591</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O56">
-        <v>0.50251470435144707</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P56">
         <v>1</v>
@@ -15486,10 +15504,10 @@
         <v>0</v>
       </c>
       <c r="N57">
-        <v>0.51018761824679415</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O57">
-        <v>0.57588816480975402</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P57">
         <v>1</v>
@@ -15539,10 +15557,10 @@
         <v>0</v>
       </c>
       <c r="N58">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O58">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P58">
         <v>1</v>
@@ -15592,10 +15610,10 @@
         <v>0</v>
       </c>
       <c r="N59">
-        <v>0.45824967357295954</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O59">
-        <v>0.51320335146725959</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P59">
         <v>1</v>
@@ -15645,10 +15663,10 @@
         <v>0</v>
       </c>
       <c r="N60">
-        <v>0.76547381653636815</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O60">
-        <v>0.62342333215136003</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P60">
         <v>1</v>
@@ -15698,10 +15716,10 @@
         <v>0</v>
       </c>
       <c r="N61">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O61">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P61">
         <v>1</v>
@@ -15751,10 +15769,10 @@
         <v>0</v>
       </c>
       <c r="N62">
-        <v>0.5183350138918108</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O62">
-        <v>0.40189685832839361</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P62">
         <v>1</v>
@@ -15804,10 +15822,10 @@
         <v>0</v>
       </c>
       <c r="N63">
-        <v>0.49311216913983535</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O63">
-        <v>0.45596609720566816</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P63">
         <v>1</v>
@@ -15857,10 +15875,10 @@
         <v>0</v>
       </c>
       <c r="N64">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O64">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P64">
         <v>1</v>
@@ -15910,10 +15928,10 @@
         <v>0</v>
       </c>
       <c r="N65">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O65">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P65">
         <v>1</v>
@@ -15963,10 +15981,10 @@
         <v>0</v>
       </c>
       <c r="N66">
-        <v>0.74238993663655861</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O66">
-        <v>0.53287461773700306</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P66">
         <v>1</v>
@@ -16016,10 +16034,10 @@
         <v>0</v>
       </c>
       <c r="N67">
-        <v>0.84562439327596528</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O67">
-        <v>0.69700323243260454</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P67">
         <v>1</v>
@@ -16069,10 +16087,10 @@
         <v>0</v>
       </c>
       <c r="N68">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O68">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P68">
         <v>1</v>
@@ -16122,10 +16140,10 @@
         <v>0</v>
       </c>
       <c r="N69">
-        <v>0.54974923912371776</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O69">
-        <v>0.39400774523132698</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P69">
         <v>1</v>
@@ -16175,10 +16193,10 @@
         <v>0</v>
       </c>
       <c r="N70">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O70">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P70">
         <v>1</v>
@@ -16228,10 +16246,10 @@
         <v>0</v>
       </c>
       <c r="N71">
-        <v>0.73426684741976689</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O71">
-        <v>0.36086076464668171</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P71">
         <v>1</v>
@@ -16281,10 +16299,10 @@
         <v>0</v>
       </c>
       <c r="N72">
-        <v>0.65139438398943228</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O72">
-        <v>0.38303397533001515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P72">
         <v>1</v>
@@ -16334,10 +16352,10 @@
         <v>0</v>
       </c>
       <c r="N73">
-        <v>0.58177137676443924</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O73">
-        <v>0.38945139302494869</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P73">
         <v>1</v>
@@ -16387,10 +16405,10 @@
         <v>0</v>
       </c>
       <c r="N74">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O74">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P74">
         <v>1</v>
@@ -16440,10 +16458,10 @@
         <v>0</v>
       </c>
       <c r="N75">
-        <v>0.35930258940223547</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O75">
-        <v>0.41103799617915515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P75">
         <v>1</v>
@@ -16493,10 +16511,10 @@
         <v>0</v>
       </c>
       <c r="N76">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O76">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P76">
         <v>1</v>
@@ -16546,10 +16564,10 @@
         <v>0</v>
       </c>
       <c r="N77">
-        <v>0.64831027719689605</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O77">
-        <v>0.62341807401314386</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P77">
         <v>1</v>
@@ -16599,10 +16617,10 @@
         <v>0</v>
       </c>
       <c r="N78">
-        <v>0.4448676725204056</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O78">
-        <v>0.41531041305960925</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P78">
         <v>1</v>
@@ -16652,10 +16670,10 @@
         <v>0</v>
       </c>
       <c r="N79">
-        <v>0.52352941176470591</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O79">
-        <v>0.50251470435144707</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P79">
         <v>1</v>
@@ -16705,10 +16723,10 @@
         <v>0</v>
       </c>
       <c r="N80">
-        <v>0.51018761824679415</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O80">
-        <v>0.57588816480975402</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P80">
         <v>1</v>
@@ -16758,10 +16776,10 @@
         <v>0</v>
       </c>
       <c r="N81">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O81">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P81">
         <v>1</v>
@@ -16811,10 +16829,10 @@
         <v>0</v>
       </c>
       <c r="N82">
-        <v>0.45824967357295954</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O82">
-        <v>0.51320335146725959</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P82">
         <v>1</v>
@@ -16864,10 +16882,10 @@
         <v>0</v>
       </c>
       <c r="N83">
-        <v>0.76547381653636815</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O83">
-        <v>0.62342333215136003</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P83">
         <v>1</v>
@@ -16917,10 +16935,10 @@
         <v>0</v>
       </c>
       <c r="N84">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O84">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P84">
         <v>1</v>
@@ -16970,10 +16988,10 @@
         <v>0</v>
       </c>
       <c r="N85">
-        <v>0.5183350138918108</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O85">
-        <v>0.40189685832839361</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P85">
         <v>1</v>
@@ -17023,10 +17041,10 @@
         <v>0</v>
       </c>
       <c r="N86">
-        <v>0.49311216913983535</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O86">
-        <v>0.45596609720566816</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P86">
         <v>1</v>
@@ -17076,10 +17094,10 @@
         <v>0</v>
       </c>
       <c r="N87">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O87">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P87">
         <v>1</v>
@@ -17129,10 +17147,10 @@
         <v>0</v>
       </c>
       <c r="N88">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O88">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P88">
         <v>1</v>
@@ -17182,10 +17200,10 @@
         <v>0</v>
       </c>
       <c r="N89">
-        <v>0.74238993663655861</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O89">
-        <v>0.53287461773700306</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P89">
         <v>1</v>
@@ -17235,10 +17253,10 @@
         <v>0</v>
       </c>
       <c r="N90">
-        <v>0.84562439327596528</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O90">
-        <v>0.69700323243260454</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P90">
         <v>1</v>
@@ -17288,10 +17306,10 @@
         <v>0</v>
       </c>
       <c r="N91">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O91">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P91">
         <v>1</v>
@@ -17341,10 +17359,10 @@
         <v>0</v>
       </c>
       <c r="N92">
-        <v>0.54974923912371776</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O92">
-        <v>0.39400774523132698</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P92">
         <v>1</v>
@@ -17394,10 +17412,10 @@
         <v>0</v>
       </c>
       <c r="N93">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O93">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P93">
         <v>1</v>
@@ -19689,10 +19707,10 @@
         <v>0</v>
       </c>
       <c r="N140">
-        <v>0.73426684741976689</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O140">
-        <v>0.36086076464668171</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P140">
         <v>1</v>
@@ -19742,10 +19760,10 @@
         <v>0</v>
       </c>
       <c r="N141">
-        <v>0.65139438398943228</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O141">
-        <v>0.38303397533001515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P141">
         <v>1</v>
@@ -19795,10 +19813,10 @@
         <v>0</v>
       </c>
       <c r="N142">
-        <v>0.58177137676443924</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O142">
-        <v>0.38945139302494869</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P142">
         <v>1</v>
@@ -19848,10 +19866,10 @@
         <v>0</v>
       </c>
       <c r="N143">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O143">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P143">
         <v>1</v>
@@ -19901,10 +19919,10 @@
         <v>0</v>
       </c>
       <c r="N144">
-        <v>0.35930258940223547</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O144">
-        <v>0.41103799617915515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P144">
         <v>1</v>
@@ -19954,10 +19972,10 @@
         <v>0</v>
       </c>
       <c r="N145">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O145">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P145">
         <v>1</v>
@@ -20007,10 +20025,10 @@
         <v>0</v>
       </c>
       <c r="N146">
-        <v>0.64831027719689605</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O146">
-        <v>0.62341807401314386</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P146">
         <v>1</v>
@@ -20060,10 +20078,10 @@
         <v>0</v>
       </c>
       <c r="N147">
-        <v>0.4448676725204056</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O147">
-        <v>0.41531041305960925</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P147">
         <v>1</v>
@@ -20113,10 +20131,10 @@
         <v>0</v>
       </c>
       <c r="N148">
-        <v>0.52352941176470591</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O148">
-        <v>0.50251470435144707</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P148">
         <v>1</v>
@@ -20166,10 +20184,10 @@
         <v>0</v>
       </c>
       <c r="N149">
-        <v>0.51018761824679415</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O149">
-        <v>0.57588816480975402</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P149">
         <v>1</v>
@@ -20219,10 +20237,10 @@
         <v>0</v>
       </c>
       <c r="N150">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O150">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P150">
         <v>1</v>
@@ -20272,10 +20290,10 @@
         <v>0</v>
       </c>
       <c r="N151">
-        <v>0.45824967357295954</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O151">
-        <v>0.51320335146725959</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P151">
         <v>1</v>
@@ -20325,10 +20343,10 @@
         <v>0</v>
       </c>
       <c r="N152">
-        <v>0.76547381653636815</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O152">
-        <v>0.62342333215136003</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P152">
         <v>1</v>
@@ -20378,10 +20396,10 @@
         <v>0</v>
       </c>
       <c r="N153">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O153">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P153">
         <v>1</v>
@@ -20431,10 +20449,10 @@
         <v>0</v>
       </c>
       <c r="N154">
-        <v>0.5183350138918108</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O154">
-        <v>0.40189685832839361</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P154">
         <v>1</v>
@@ -20484,10 +20502,10 @@
         <v>0</v>
       </c>
       <c r="N155">
-        <v>0.49311216913983535</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O155">
-        <v>0.45596609720566816</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P155">
         <v>1</v>
@@ -20537,10 +20555,10 @@
         <v>0</v>
       </c>
       <c r="N156">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O156">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P156">
         <v>1</v>
@@ -20590,10 +20608,10 @@
         <v>0</v>
       </c>
       <c r="N157">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O157">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P157">
         <v>1</v>
@@ -20643,10 +20661,10 @@
         <v>0</v>
       </c>
       <c r="N158">
-        <v>0.74238993663655861</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O158">
-        <v>0.53287461773700306</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P158">
         <v>1</v>
@@ -20696,10 +20714,10 @@
         <v>0</v>
       </c>
       <c r="N159">
-        <v>0.84562439327596528</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O159">
-        <v>0.69700323243260454</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P159">
         <v>1</v>
@@ -20749,10 +20767,10 @@
         <v>0</v>
       </c>
       <c r="N160">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O160">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P160">
         <v>1</v>
@@ -20802,10 +20820,10 @@
         <v>0</v>
       </c>
       <c r="N161">
-        <v>0.54974923912371776</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O161">
-        <v>0.39400774523132698</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P161">
         <v>1</v>
@@ -20855,10 +20873,10 @@
         <v>0</v>
       </c>
       <c r="N162">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O162">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P162">
         <v>1</v>
@@ -20908,10 +20926,10 @@
         <v>0</v>
       </c>
       <c r="N163">
-        <v>0.73426684741976689</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O163">
-        <v>0.36086076464668171</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P163">
         <v>1</v>
@@ -20961,10 +20979,10 @@
         <v>0</v>
       </c>
       <c r="N164">
-        <v>0.65139438398943228</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O164">
-        <v>0.38303397533001515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P164">
         <v>1</v>
@@ -21014,10 +21032,10 @@
         <v>0</v>
       </c>
       <c r="N165">
-        <v>0.58177137676443924</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O165">
-        <v>0.38945139302494869</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P165">
         <v>1</v>
@@ -21067,10 +21085,10 @@
         <v>0</v>
       </c>
       <c r="N166">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O166">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P166">
         <v>1</v>
@@ -21120,10 +21138,10 @@
         <v>0</v>
       </c>
       <c r="N167">
-        <v>0.35930258940223547</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O167">
-        <v>0.41103799617915515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P167">
         <v>1</v>
@@ -21173,10 +21191,10 @@
         <v>0</v>
       </c>
       <c r="N168">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O168">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P168">
         <v>1</v>
@@ -21226,10 +21244,10 @@
         <v>0</v>
       </c>
       <c r="N169">
-        <v>0.64831027719689605</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O169">
-        <v>0.62341807401314386</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P169">
         <v>1</v>
@@ -21279,10 +21297,10 @@
         <v>0</v>
       </c>
       <c r="N170">
-        <v>0.4448676725204056</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O170">
-        <v>0.41531041305960925</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P170">
         <v>1</v>
@@ -21332,10 +21350,10 @@
         <v>0</v>
       </c>
       <c r="N171">
-        <v>0.52352941176470591</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O171">
-        <v>0.50251470435144707</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P171">
         <v>1</v>
@@ -21385,10 +21403,10 @@
         <v>0</v>
       </c>
       <c r="N172">
-        <v>0.51018761824679415</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O172">
-        <v>0.57588816480975402</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P172">
         <v>1</v>
@@ -21438,10 +21456,10 @@
         <v>0</v>
       </c>
       <c r="N173">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O173">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P173">
         <v>1</v>
@@ -21491,10 +21509,10 @@
         <v>0</v>
       </c>
       <c r="N174">
-        <v>0.45824967357295954</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O174">
-        <v>0.51320335146725959</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P174">
         <v>1</v>
@@ -21544,10 +21562,10 @@
         <v>0</v>
       </c>
       <c r="N175">
-        <v>0.76547381653636815</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O175">
-        <v>0.62342333215136003</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P175">
         <v>1</v>
@@ -21597,10 +21615,10 @@
         <v>0</v>
       </c>
       <c r="N176">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O176">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P176">
         <v>1</v>
@@ -21650,10 +21668,10 @@
         <v>0</v>
       </c>
       <c r="N177">
-        <v>0.5183350138918108</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O177">
-        <v>0.40189685832839361</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P177">
         <v>1</v>
@@ -21703,10 +21721,10 @@
         <v>0</v>
       </c>
       <c r="N178">
-        <v>0.49311216913983535</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O178">
-        <v>0.45596609720566816</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P178">
         <v>1</v>
@@ -21756,10 +21774,10 @@
         <v>0</v>
       </c>
       <c r="N179">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O179">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P179">
         <v>1</v>
@@ -21809,10 +21827,10 @@
         <v>0</v>
       </c>
       <c r="N180">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O180">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P180">
         <v>1</v>
@@ -21862,10 +21880,10 @@
         <v>0</v>
       </c>
       <c r="N181">
-        <v>0.74238993663655861</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O181">
-        <v>0.53287461773700306</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P181">
         <v>1</v>
@@ -21915,10 +21933,10 @@
         <v>0</v>
       </c>
       <c r="N182">
-        <v>0.84562439327596528</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O182">
-        <v>0.69700323243260454</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P182">
         <v>1</v>
@@ -21968,10 +21986,10 @@
         <v>0</v>
       </c>
       <c r="N183">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O183">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P183">
         <v>1</v>
@@ -22021,10 +22039,10 @@
         <v>0</v>
       </c>
       <c r="N184">
-        <v>0.54974923912371776</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O184">
-        <v>0.39400774523132698</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P184">
         <v>1</v>
@@ -22074,10 +22092,10 @@
         <v>0</v>
       </c>
       <c r="N185">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O185">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P185">
         <v>1</v>
@@ -22127,10 +22145,10 @@
         <v>0</v>
       </c>
       <c r="N186">
-        <v>0.73426684741976689</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O186">
-        <v>0.36086076464668171</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P186">
         <v>1</v>
@@ -22180,10 +22198,10 @@
         <v>0</v>
       </c>
       <c r="N187">
-        <v>0.65139438398943228</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O187">
-        <v>0.38303397533001515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P187">
         <v>1</v>
@@ -22233,10 +22251,10 @@
         <v>0</v>
       </c>
       <c r="N188">
-        <v>0.58177137676443924</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O188">
-        <v>0.38945139302494869</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P188">
         <v>1</v>
@@ -22286,10 +22304,10 @@
         <v>0</v>
       </c>
       <c r="N189">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O189">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P189">
         <v>1</v>
@@ -22339,10 +22357,10 @@
         <v>0</v>
       </c>
       <c r="N190">
-        <v>0.35930258940223547</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O190">
-        <v>0.41103799617915515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P190">
         <v>1</v>
@@ -22392,10 +22410,10 @@
         <v>0</v>
       </c>
       <c r="N191">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O191">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P191">
         <v>1</v>
@@ -22445,10 +22463,10 @@
         <v>0</v>
       </c>
       <c r="N192">
-        <v>0.64831027719689605</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O192">
-        <v>0.62341807401314386</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P192">
         <v>1</v>
@@ -22498,10 +22516,10 @@
         <v>0</v>
       </c>
       <c r="N193">
-        <v>0.4448676725204056</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O193">
-        <v>0.41531041305960925</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P193">
         <v>1</v>
@@ -22551,10 +22569,10 @@
         <v>0</v>
       </c>
       <c r="N194">
-        <v>0.52352941176470591</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O194">
-        <v>0.50251470435144707</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P194">
         <v>1</v>
@@ -22604,10 +22622,10 @@
         <v>0</v>
       </c>
       <c r="N195">
-        <v>0.51018761824679415</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O195">
-        <v>0.57588816480975402</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P195">
         <v>1</v>
@@ -22657,10 +22675,10 @@
         <v>0</v>
       </c>
       <c r="N196">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O196">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P196">
         <v>1</v>
@@ -22710,10 +22728,10 @@
         <v>0</v>
       </c>
       <c r="N197">
-        <v>0.45824967357295954</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O197">
-        <v>0.51320335146725959</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P197">
         <v>1</v>
@@ -22763,10 +22781,10 @@
         <v>0</v>
       </c>
       <c r="N198">
-        <v>0.76547381653636815</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O198">
-        <v>0.62342333215136003</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P198">
         <v>1</v>
@@ -22816,10 +22834,10 @@
         <v>0</v>
       </c>
       <c r="N199">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O199">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P199">
         <v>1</v>
@@ -22869,10 +22887,10 @@
         <v>0</v>
       </c>
       <c r="N200">
-        <v>0.5183350138918108</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O200">
-        <v>0.40189685832839361</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P200">
         <v>1</v>
@@ -22922,10 +22940,10 @@
         <v>0</v>
       </c>
       <c r="N201">
-        <v>0.49311216913983535</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O201">
-        <v>0.45596609720566816</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P201">
         <v>1</v>
@@ -22975,10 +22993,10 @@
         <v>0</v>
       </c>
       <c r="N202">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O202">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P202">
         <v>1</v>
@@ -23028,10 +23046,10 @@
         <v>0</v>
       </c>
       <c r="N203">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O203">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P203">
         <v>1</v>
@@ -23081,10 +23099,10 @@
         <v>0</v>
       </c>
       <c r="N204">
-        <v>0.74238993663655861</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O204">
-        <v>0.53287461773700306</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P204">
         <v>1</v>
@@ -23134,10 +23152,10 @@
         <v>0</v>
       </c>
       <c r="N205">
-        <v>0.84562439327596528</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O205">
-        <v>0.69700323243260454</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P205">
         <v>1</v>
@@ -23187,10 +23205,10 @@
         <v>0</v>
       </c>
       <c r="N206">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O206">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P206">
         <v>1</v>
@@ -23240,10 +23258,10 @@
         <v>0</v>
       </c>
       <c r="N207">
-        <v>0.54974923912371776</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O207">
-        <v>0.39400774523132698</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P207">
         <v>1</v>
@@ -23293,10 +23311,10 @@
         <v>0</v>
       </c>
       <c r="N208">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O208">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P208">
         <v>1</v>
@@ -23346,10 +23364,10 @@
         <v>0</v>
       </c>
       <c r="N209">
-        <v>0.73426684741976689</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O209">
-        <v>0.36086076464668171</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P209">
         <v>1</v>
@@ -23399,10 +23417,10 @@
         <v>0</v>
       </c>
       <c r="N210">
-        <v>0.65139438398943228</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O210">
-        <v>0.38303397533001515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P210">
         <v>1</v>
@@ -23452,10 +23470,10 @@
         <v>0</v>
       </c>
       <c r="N211">
-        <v>0.58177137676443924</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O211">
-        <v>0.38945139302494869</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P211">
         <v>1</v>
@@ -23505,10 +23523,10 @@
         <v>0</v>
       </c>
       <c r="N212">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O212">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P212">
         <v>1</v>
@@ -23558,10 +23576,10 @@
         <v>0</v>
       </c>
       <c r="N213">
-        <v>0.35930258940223547</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O213">
-        <v>0.41103799617915515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P213">
         <v>1</v>
@@ -23611,10 +23629,10 @@
         <v>0</v>
       </c>
       <c r="N214">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O214">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P214">
         <v>1</v>
@@ -23664,10 +23682,10 @@
         <v>0</v>
       </c>
       <c r="N215">
-        <v>0.64831027719689605</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O215">
-        <v>0.62341807401314386</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P215">
         <v>1</v>
@@ -23717,10 +23735,10 @@
         <v>0</v>
       </c>
       <c r="N216">
-        <v>0.4448676725204056</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O216">
-        <v>0.41531041305960925</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P216">
         <v>1</v>
@@ -23770,10 +23788,10 @@
         <v>0</v>
       </c>
       <c r="N217">
-        <v>0.52352941176470591</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O217">
-        <v>0.50251470435144707</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P217">
         <v>1</v>
@@ -23823,10 +23841,10 @@
         <v>0</v>
       </c>
       <c r="N218">
-        <v>0.51018761824679415</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O218">
-        <v>0.57588816480975402</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P218">
         <v>1</v>
@@ -23876,10 +23894,10 @@
         <v>0</v>
       </c>
       <c r="N219">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O219">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P219">
         <v>1</v>
@@ -23929,10 +23947,10 @@
         <v>0</v>
       </c>
       <c r="N220">
-        <v>0.45824967357295954</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O220">
-        <v>0.51320335146725959</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P220">
         <v>1</v>
@@ -23982,10 +24000,10 @@
         <v>0</v>
       </c>
       <c r="N221">
-        <v>0.76547381653636815</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O221">
-        <v>0.62342333215136003</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P221">
         <v>1</v>
@@ -24035,10 +24053,10 @@
         <v>0</v>
       </c>
       <c r="N222">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O222">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P222">
         <v>1</v>
@@ -24088,10 +24106,10 @@
         <v>0</v>
       </c>
       <c r="N223">
-        <v>0.5183350138918108</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O223">
-        <v>0.40189685832839361</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P223">
         <v>1</v>
@@ -24141,10 +24159,10 @@
         <v>0</v>
       </c>
       <c r="N224">
-        <v>0.49311216913983535</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O224">
-        <v>0.45596609720566816</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P224">
         <v>1</v>
@@ -24194,10 +24212,10 @@
         <v>0</v>
       </c>
       <c r="N225">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O225">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P225">
         <v>1</v>
@@ -24247,10 +24265,10 @@
         <v>0</v>
       </c>
       <c r="N226">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O226">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P226">
         <v>1</v>
@@ -24300,10 +24318,10 @@
         <v>0</v>
       </c>
       <c r="N227">
-        <v>0.74238993663655861</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O227">
-        <v>0.53287461773700306</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P227">
         <v>1</v>
@@ -24353,10 +24371,10 @@
         <v>0</v>
       </c>
       <c r="N228">
-        <v>0.84562439327596528</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O228">
-        <v>0.69700323243260454</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P228">
         <v>1</v>
@@ -24406,10 +24424,10 @@
         <v>0</v>
       </c>
       <c r="N229">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O229">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P229">
         <v>1</v>
@@ -24459,10 +24477,10 @@
         <v>0</v>
       </c>
       <c r="N230">
-        <v>0.54974923912371776</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O230">
-        <v>0.39400774523132698</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P230">
         <v>1</v>
@@ -24512,10 +24530,10 @@
         <v>0</v>
       </c>
       <c r="N231">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O231">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P231">
         <v>1</v>
@@ -24565,10 +24583,10 @@
         <v>0</v>
       </c>
       <c r="N232">
-        <v>0.73426684741976689</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O232">
-        <v>0.36086076464668171</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P232">
         <v>1</v>
@@ -24618,10 +24636,10 @@
         <v>0</v>
       </c>
       <c r="N233">
-        <v>0.65139438398943228</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O233">
-        <v>0.38303397533001515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P233">
         <v>1</v>
@@ -24671,10 +24689,10 @@
         <v>0</v>
       </c>
       <c r="N234">
-        <v>0.58177137676443924</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O234">
-        <v>0.38945139302494869</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P234">
         <v>1</v>
@@ -24724,10 +24742,10 @@
         <v>0</v>
       </c>
       <c r="N235">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O235">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P235">
         <v>1</v>
@@ -24777,10 +24795,10 @@
         <v>0</v>
       </c>
       <c r="N236">
-        <v>0.35930258940223547</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O236">
-        <v>0.41103799617915515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P236">
         <v>1</v>
@@ -24830,10 +24848,10 @@
         <v>0</v>
       </c>
       <c r="N237">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O237">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P237">
         <v>1</v>
@@ -24883,10 +24901,10 @@
         <v>0</v>
       </c>
       <c r="N238">
-        <v>0.64831027719689605</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O238">
-        <v>0.62341807401314386</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P238">
         <v>1</v>
@@ -24936,10 +24954,10 @@
         <v>0</v>
       </c>
       <c r="N239">
-        <v>0.4448676725204056</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O239">
-        <v>0.41531041305960925</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P239">
         <v>1</v>
@@ -24989,10 +25007,10 @@
         <v>0</v>
       </c>
       <c r="N240">
-        <v>0.52352941176470591</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O240">
-        <v>0.50251470435144707</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P240">
         <v>1</v>
@@ -25042,10 +25060,10 @@
         <v>0</v>
       </c>
       <c r="N241">
-        <v>0.51018761824679415</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O241">
-        <v>0.57588816480975402</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P241">
         <v>1</v>
@@ -25095,10 +25113,10 @@
         <v>0</v>
       </c>
       <c r="N242">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O242">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P242">
         <v>1</v>
@@ -25148,10 +25166,10 @@
         <v>0</v>
       </c>
       <c r="N243">
-        <v>0.45824967357295954</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O243">
-        <v>0.51320335146725959</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P243">
         <v>1</v>
@@ -25201,10 +25219,10 @@
         <v>0</v>
       </c>
       <c r="N244">
-        <v>0.76547381653636815</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O244">
-        <v>0.62342333215136003</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P244">
         <v>1</v>
@@ -25254,10 +25272,10 @@
         <v>0</v>
       </c>
       <c r="N245">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O245">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P245">
         <v>1</v>
@@ -25307,10 +25325,10 @@
         <v>0</v>
       </c>
       <c r="N246">
-        <v>0.5183350138918108</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O246">
-        <v>0.40189685832839361</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P246">
         <v>1</v>
@@ -25360,10 +25378,10 @@
         <v>0</v>
       </c>
       <c r="N247">
-        <v>0.49311216913983535</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O247">
-        <v>0.45596609720566816</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P247">
         <v>1</v>
@@ -25413,10 +25431,10 @@
         <v>0</v>
       </c>
       <c r="N248">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O248">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P248">
         <v>1</v>
@@ -25466,10 +25484,10 @@
         <v>0</v>
       </c>
       <c r="N249">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O249">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P249">
         <v>1</v>
@@ -25519,10 +25537,10 @@
         <v>0</v>
       </c>
       <c r="N250">
-        <v>0.74238993663655861</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O250">
-        <v>0.53287461773700306</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P250">
         <v>1</v>
@@ -25572,10 +25590,10 @@
         <v>0</v>
       </c>
       <c r="N251">
-        <v>0.84562439327596528</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O251">
-        <v>0.69700323243260454</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P251">
         <v>1</v>
@@ -25625,10 +25643,10 @@
         <v>0</v>
       </c>
       <c r="N252">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O252">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P252">
         <v>1</v>
@@ -25678,10 +25696,10 @@
         <v>0</v>
       </c>
       <c r="N253">
-        <v>0.54974923912371776</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O253">
-        <v>0.39400774523132698</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P253">
         <v>1</v>
@@ -25731,10 +25749,10 @@
         <v>0</v>
       </c>
       <c r="N254">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O254">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P254">
         <v>1</v>
@@ -25784,10 +25802,10 @@
         <v>0</v>
       </c>
       <c r="N255">
-        <v>0.73426684741976689</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O255">
-        <v>0.36086076464668171</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P255">
         <v>1</v>
@@ -25837,10 +25855,10 @@
         <v>0</v>
       </c>
       <c r="N256">
-        <v>0.65139438398943228</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O256">
-        <v>0.38303397533001515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P256">
         <v>1</v>
@@ -25890,10 +25908,10 @@
         <v>0</v>
       </c>
       <c r="N257">
-        <v>0.58177137676443924</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O257">
-        <v>0.38945139302494869</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P257">
         <v>1</v>
@@ -25943,10 +25961,10 @@
         <v>0</v>
       </c>
       <c r="N258">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O258">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P258">
         <v>1</v>
@@ -25996,10 +26014,10 @@
         <v>0</v>
       </c>
       <c r="N259">
-        <v>0.35930258940223547</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O259">
-        <v>0.41103799617915515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P259">
         <v>1</v>
@@ -26049,10 +26067,10 @@
         <v>0</v>
       </c>
       <c r="N260">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O260">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P260">
         <v>1</v>
@@ -26102,10 +26120,10 @@
         <v>0</v>
       </c>
       <c r="N261">
-        <v>0.64831027719689605</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O261">
-        <v>0.62341807401314386</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P261">
         <v>1</v>
@@ -26155,10 +26173,10 @@
         <v>0</v>
       </c>
       <c r="N262">
-        <v>0.4448676725204056</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O262">
-        <v>0.41531041305960925</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P262">
         <v>1</v>
@@ -26208,10 +26226,10 @@
         <v>0</v>
       </c>
       <c r="N263">
-        <v>0.52352941176470591</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O263">
-        <v>0.50251470435144707</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P263">
         <v>1</v>
@@ -26261,10 +26279,10 @@
         <v>0</v>
       </c>
       <c r="N264">
-        <v>0.51018761824679415</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O264">
-        <v>0.57588816480975402</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P264">
         <v>1</v>
@@ -26314,10 +26332,10 @@
         <v>0</v>
       </c>
       <c r="N265">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O265">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P265">
         <v>1</v>
@@ -26367,10 +26385,10 @@
         <v>0</v>
       </c>
       <c r="N266">
-        <v>0.45824967357295954</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O266">
-        <v>0.51320335146725959</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P266">
         <v>1</v>
@@ -26420,10 +26438,10 @@
         <v>0</v>
       </c>
       <c r="N267">
-        <v>0.76547381653636815</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O267">
-        <v>0.62342333215136003</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P267">
         <v>1</v>
@@ -26473,10 +26491,10 @@
         <v>0</v>
       </c>
       <c r="N268">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O268">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P268">
         <v>1</v>
@@ -26526,10 +26544,10 @@
         <v>0</v>
       </c>
       <c r="N269">
-        <v>0.5183350138918108</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O269">
-        <v>0.40189685832839361</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P269">
         <v>1</v>
@@ -26579,10 +26597,10 @@
         <v>0</v>
       </c>
       <c r="N270">
-        <v>0.49311216913983535</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O270">
-        <v>0.45596609720566816</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P270">
         <v>1</v>
@@ -26632,10 +26650,10 @@
         <v>0</v>
       </c>
       <c r="N271">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O271">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P271">
         <v>1</v>
@@ -26685,10 +26703,10 @@
         <v>0</v>
       </c>
       <c r="N272">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O272">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P272">
         <v>1</v>
@@ -26738,10 +26756,10 @@
         <v>0</v>
       </c>
       <c r="N273">
-        <v>0.74238993663655861</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O273">
-        <v>0.53287461773700306</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P273">
         <v>1</v>
@@ -26791,10 +26809,10 @@
         <v>0</v>
       </c>
       <c r="N274">
-        <v>0.84562439327596528</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O274">
-        <v>0.69700323243260454</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P274">
         <v>1</v>
@@ -26844,10 +26862,10 @@
         <v>0</v>
       </c>
       <c r="N275">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O275">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P275">
         <v>1</v>
@@ -26897,10 +26915,10 @@
         <v>0</v>
       </c>
       <c r="N276">
-        <v>0.54974923912371776</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O276">
-        <v>0.39400774523132698</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P276">
         <v>1</v>
@@ -26950,10 +26968,10 @@
         <v>0</v>
       </c>
       <c r="N277">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O277">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P277">
         <v>1</v>
@@ -28222,10 +28240,10 @@
         <v>0</v>
       </c>
       <c r="N301">
-        <v>0.73426684741976689</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O301">
-        <v>0.36086076464668171</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P301">
         <v>1</v>
@@ -28275,10 +28293,10 @@
         <v>0</v>
       </c>
       <c r="N302">
-        <v>0.65139438398943228</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O302">
-        <v>0.38303397533001515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P302">
         <v>1</v>
@@ -28328,10 +28346,10 @@
         <v>0</v>
       </c>
       <c r="N303">
-        <v>0.58177137676443924</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O303">
-        <v>0.38945139302494869</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P303">
         <v>1</v>
@@ -28381,10 +28399,10 @@
         <v>0</v>
       </c>
       <c r="N304">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O304">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P304">
         <v>1</v>
@@ -28434,10 +28452,10 @@
         <v>0</v>
       </c>
       <c r="N305">
-        <v>0.35930258940223547</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O305">
-        <v>0.41103799617915515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P305">
         <v>1</v>
@@ -28487,10 +28505,10 @@
         <v>0</v>
       </c>
       <c r="N306">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O306">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P306">
         <v>1</v>
@@ -28540,10 +28558,10 @@
         <v>0</v>
       </c>
       <c r="N307">
-        <v>0.64831027719689605</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O307">
-        <v>0.62341807401314386</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P307">
         <v>1</v>
@@ -28593,10 +28611,10 @@
         <v>0</v>
       </c>
       <c r="N308">
-        <v>0.4448676725204056</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O308">
-        <v>0.41531041305960925</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P308">
         <v>1</v>
@@ -28646,10 +28664,10 @@
         <v>0</v>
       </c>
       <c r="N309">
-        <v>0.52352941176470591</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O309">
-        <v>0.50251470435144707</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P309">
         <v>1</v>
@@ -28699,10 +28717,10 @@
         <v>0</v>
       </c>
       <c r="N310">
-        <v>0.51018761824679415</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O310">
-        <v>0.57588816480975402</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P310">
         <v>1</v>
@@ -28752,10 +28770,10 @@
         <v>0</v>
       </c>
       <c r="N311">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O311">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P311">
         <v>1</v>
@@ -28805,10 +28823,10 @@
         <v>0</v>
       </c>
       <c r="N312">
-        <v>0.45824967357295954</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O312">
-        <v>0.51320335146725959</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P312">
         <v>1</v>
@@ -28858,10 +28876,10 @@
         <v>0</v>
       </c>
       <c r="N313">
-        <v>0.76547381653636815</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O313">
-        <v>0.62342333215136003</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P313">
         <v>1</v>
@@ -28911,10 +28929,10 @@
         <v>0</v>
       </c>
       <c r="N314">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O314">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P314">
         <v>1</v>
@@ -28964,10 +28982,10 @@
         <v>0</v>
       </c>
       <c r="N315">
-        <v>0.5183350138918108</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O315">
-        <v>0.40189685832839361</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P315">
         <v>1</v>
@@ -29017,10 +29035,10 @@
         <v>0</v>
       </c>
       <c r="N316">
-        <v>0.49311216913983535</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O316">
-        <v>0.45596609720566816</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P316">
         <v>1</v>
@@ -29070,10 +29088,10 @@
         <v>0</v>
       </c>
       <c r="N317">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O317">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P317">
         <v>1</v>
@@ -29123,10 +29141,10 @@
         <v>0</v>
       </c>
       <c r="N318">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O318">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P318">
         <v>1</v>
@@ -29176,10 +29194,10 @@
         <v>0</v>
       </c>
       <c r="N319">
-        <v>0.74238993663655861</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O319">
-        <v>0.53287461773700306</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P319">
         <v>1</v>
@@ -29229,10 +29247,10 @@
         <v>0</v>
       </c>
       <c r="N320">
-        <v>0.84562439327596528</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O320">
-        <v>0.69700323243260454</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P320">
         <v>1</v>
@@ -29282,10 +29300,10 @@
         <v>0</v>
       </c>
       <c r="N321">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O321">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P321">
         <v>1</v>
@@ -29335,10 +29353,10 @@
         <v>0</v>
       </c>
       <c r="N322">
-        <v>0.54974923912371776</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O322">
-        <v>0.39400774523132698</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P322">
         <v>1</v>
@@ -29388,10 +29406,10 @@
         <v>0</v>
       </c>
       <c r="N323">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O323">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P323">
         <v>1</v>
@@ -29441,10 +29459,10 @@
         <v>0</v>
       </c>
       <c r="N324">
-        <v>0.73426684741976689</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O324">
-        <v>0.36086076464668171</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P324">
         <v>1</v>
@@ -29494,10 +29512,10 @@
         <v>0</v>
       </c>
       <c r="N325">
-        <v>0.65139438398943228</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O325">
-        <v>0.38303397533001515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P325">
         <v>1</v>
@@ -29547,10 +29565,10 @@
         <v>0</v>
       </c>
       <c r="N326">
-        <v>0.58177137676443924</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O326">
-        <v>0.38945139302494869</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P326">
         <v>1</v>
@@ -29600,10 +29618,10 @@
         <v>0</v>
       </c>
       <c r="N327">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O327">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P327">
         <v>1</v>
@@ -29653,10 +29671,10 @@
         <v>0</v>
       </c>
       <c r="N328">
-        <v>0.35930258940223547</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O328">
-        <v>0.41103799617915515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P328">
         <v>1</v>
@@ -29706,10 +29724,10 @@
         <v>0</v>
       </c>
       <c r="N329">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O329">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P329">
         <v>1</v>
@@ -29759,10 +29777,10 @@
         <v>0</v>
       </c>
       <c r="N330">
-        <v>0.64831027719689605</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O330">
-        <v>0.62341807401314386</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P330">
         <v>1</v>
@@ -29812,10 +29830,10 @@
         <v>0</v>
       </c>
       <c r="N331">
-        <v>0.4448676725204056</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O331">
-        <v>0.41531041305960925</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P331">
         <v>1</v>
@@ -29865,10 +29883,10 @@
         <v>0</v>
       </c>
       <c r="N332">
-        <v>0.52352941176470591</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O332">
-        <v>0.50251470435144707</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P332">
         <v>1</v>
@@ -29918,10 +29936,10 @@
         <v>0</v>
       </c>
       <c r="N333">
-        <v>0.51018761824679415</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O333">
-        <v>0.57588816480975402</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P333">
         <v>1</v>
@@ -29971,10 +29989,10 @@
         <v>0</v>
       </c>
       <c r="N334">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O334">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P334">
         <v>1</v>
@@ -30024,10 +30042,10 @@
         <v>0</v>
       </c>
       <c r="N335">
-        <v>0.45824967357295954</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O335">
-        <v>0.51320335146725959</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P335">
         <v>1</v>
@@ -30077,10 +30095,10 @@
         <v>0</v>
       </c>
       <c r="N336">
-        <v>0.76547381653636815</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O336">
-        <v>0.62342333215136003</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P336">
         <v>1</v>
@@ -30130,10 +30148,10 @@
         <v>0</v>
       </c>
       <c r="N337">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O337">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P337">
         <v>1</v>
@@ -30183,10 +30201,10 @@
         <v>0</v>
       </c>
       <c r="N338">
-        <v>0.5183350138918108</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O338">
-        <v>0.40189685832839361</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P338">
         <v>1</v>
@@ -30236,10 +30254,10 @@
         <v>0</v>
       </c>
       <c r="N339">
-        <v>0.49311216913983535</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O339">
-        <v>0.45596609720566816</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P339">
         <v>1</v>
@@ -30289,10 +30307,10 @@
         <v>0</v>
       </c>
       <c r="N340">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O340">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P340">
         <v>1</v>
@@ -30342,10 +30360,10 @@
         <v>0</v>
       </c>
       <c r="N341">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O341">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P341">
         <v>1</v>
@@ -30395,10 +30413,10 @@
         <v>0</v>
       </c>
       <c r="N342">
-        <v>0.74238993663655861</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O342">
-        <v>0.53287461773700306</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P342">
         <v>1</v>
@@ -30448,10 +30466,10 @@
         <v>0</v>
       </c>
       <c r="N343">
-        <v>0.84562439327596528</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O343">
-        <v>0.69700323243260454</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P343">
         <v>1</v>
@@ -30501,10 +30519,10 @@
         <v>0</v>
       </c>
       <c r="N344">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O344">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P344">
         <v>1</v>
@@ -30554,10 +30572,10 @@
         <v>0</v>
       </c>
       <c r="N345">
-        <v>0.54974923912371776</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O345">
-        <v>0.39400774523132698</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P345">
         <v>1</v>
@@ -30607,10 +30625,10 @@
         <v>0</v>
       </c>
       <c r="N346">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O346">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P346">
         <v>1</v>
@@ -30660,10 +30678,10 @@
         <v>0</v>
       </c>
       <c r="N347">
-        <v>0.73426684741976689</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O347">
-        <v>0.36086076464668171</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P347">
         <v>1</v>
@@ -30713,10 +30731,10 @@
         <v>0</v>
       </c>
       <c r="N348">
-        <v>0.65139438398943228</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O348">
-        <v>0.38303397533001515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P348">
         <v>1</v>
@@ -30766,10 +30784,10 @@
         <v>0</v>
       </c>
       <c r="N349">
-        <v>0.58177137676443924</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O349">
-        <v>0.38945139302494869</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P349">
         <v>1</v>
@@ -30819,10 +30837,10 @@
         <v>0</v>
       </c>
       <c r="N350">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O350">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P350">
         <v>1</v>
@@ -30872,10 +30890,10 @@
         <v>0</v>
       </c>
       <c r="N351">
-        <v>0.35930258940223547</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O351">
-        <v>0.41103799617915515</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P351">
         <v>1</v>
@@ -30925,10 +30943,10 @@
         <v>0</v>
       </c>
       <c r="N352">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O352">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P352">
         <v>1</v>
@@ -30978,10 +30996,10 @@
         <v>0</v>
       </c>
       <c r="N353">
-        <v>0.64831027719689605</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O353">
-        <v>0.62341807401314386</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P353">
         <v>1</v>
@@ -31031,10 +31049,10 @@
         <v>0</v>
       </c>
       <c r="N354">
-        <v>0.4448676725204056</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O354">
-        <v>0.41531041305960925</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P354">
         <v>1</v>
@@ -31084,10 +31102,10 @@
         <v>0</v>
       </c>
       <c r="N355">
-        <v>0.52352941176470591</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O355">
-        <v>0.50251470435144707</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P355">
         <v>1</v>
@@ -31137,10 +31155,10 @@
         <v>0</v>
       </c>
       <c r="N356">
-        <v>0.51018761824679415</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O356">
-        <v>0.57588816480975402</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P356">
         <v>1</v>
@@ -31190,10 +31208,10 @@
         <v>0</v>
       </c>
       <c r="N357">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O357">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P357">
         <v>1</v>
@@ -31243,10 +31261,10 @@
         <v>0</v>
       </c>
       <c r="N358">
-        <v>0.45824967357295954</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O358">
-        <v>0.51320335146725959</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P358">
         <v>1</v>
@@ -31296,10 +31314,10 @@
         <v>0</v>
       </c>
       <c r="N359">
-        <v>0.76547381653636815</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O359">
-        <v>0.62342333215136003</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P359">
         <v>1</v>
@@ -31349,10 +31367,10 @@
         <v>0</v>
       </c>
       <c r="N360">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O360">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P360">
         <v>1</v>
@@ -31402,10 +31420,10 @@
         <v>0</v>
       </c>
       <c r="N361">
-        <v>0.5183350138918108</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O361">
-        <v>0.40189685832839361</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P361">
         <v>1</v>
@@ -31455,10 +31473,10 @@
         <v>0</v>
       </c>
       <c r="N362">
-        <v>0.49311216913983535</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O362">
-        <v>0.45596609720566816</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P362">
         <v>1</v>
@@ -31508,10 +31526,10 @@
         <v>0</v>
       </c>
       <c r="N363">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O363">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P363">
         <v>1</v>
@@ -31561,10 +31579,10 @@
         <v>0</v>
       </c>
       <c r="N364">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O364">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P364">
         <v>1</v>
@@ -31614,10 +31632,10 @@
         <v>0</v>
       </c>
       <c r="N365">
-        <v>0.74238993663655861</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O365">
-        <v>0.53287461773700306</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P365">
         <v>1</v>
@@ -31667,10 +31685,10 @@
         <v>0</v>
       </c>
       <c r="N366">
-        <v>0.84562439327596528</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O366">
-        <v>0.69700323243260454</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P366">
         <v>1</v>
@@ -31720,10 +31738,10 @@
         <v>0</v>
       </c>
       <c r="N367">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O367">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P367">
         <v>1</v>
@@ -31773,10 +31791,10 @@
         <v>0</v>
       </c>
       <c r="N368">
-        <v>0.54974923912371776</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O368">
-        <v>0.39400774523132698</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P368">
         <v>1</v>
@@ -31826,10 +31844,10 @@
         <v>0</v>
       </c>
       <c r="N369">
-        <v>0.58843762796545951</v>
+        <v>0.38375506172839502</v>
       </c>
       <c r="O369">
-        <v>0.48532604799789142</v>
+        <v>0.24409393390000389</v>
       </c>
       <c r="P369">
         <v>1</v>
@@ -40038,7 +40056,7 @@
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>